<commit_message>
add some command and APIs,update system document
</commit_message>
<xml_diff>
--- a/新kal文件结构标准.xlsx
+++ b/新kal文件结构标准.xlsx
@@ -10,7 +10,7 @@
   </mc:AlternateContent>
   <xr:revisionPtr revIDLastSave="47" documentId="8_{A534CA01-0568-4866-92AB-63D7374C1734}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{E2711F94-9492-42EE-98EF-C7BA5D0CEC81}"/>
   <bookViews>
-    <workbookView minimized="1" xWindow="690" yWindow="3270" windowWidth="19680" windowHeight="11490" xr2:uid="{DD6A80C7-1AD5-4653-9312-6C8DBD5F89BC}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15975" xr2:uid="{DD6A80C7-1AD5-4653-9312-6C8DBD5F89BC}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -324,16 +324,16 @@
     <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="2" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="4" borderId="0" xfId="3" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="2" applyAlignment="1">
@@ -659,7 +659,7 @@
   <dimension ref="A1:Q18"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="O26" sqref="O26"/>
+      <selection activeCell="A19" sqref="A19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -668,25 +668,25 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="A1" s="4" t="s">
+      <c r="A1" s="3" t="s">
         <v>45</v>
       </c>
-      <c r="B1" s="4"/>
-      <c r="C1" s="4"/>
-      <c r="D1" s="4"/>
-      <c r="E1" s="4"/>
-      <c r="F1" s="4"/>
-      <c r="G1" s="4"/>
-      <c r="H1" s="4"/>
-      <c r="I1" s="4"/>
-      <c r="J1" s="4"/>
-      <c r="K1" s="4"/>
-      <c r="L1" s="4"/>
-      <c r="M1" s="4"/>
-      <c r="N1" s="4"/>
-      <c r="O1" s="4"/>
-      <c r="P1" s="4"/>
-      <c r="Q1" s="4"/>
+      <c r="B1" s="3"/>
+      <c r="C1" s="3"/>
+      <c r="D1" s="3"/>
+      <c r="E1" s="3"/>
+      <c r="F1" s="3"/>
+      <c r="G1" s="3"/>
+      <c r="H1" s="3"/>
+      <c r="I1" s="3"/>
+      <c r="J1" s="3"/>
+      <c r="K1" s="3"/>
+      <c r="L1" s="3"/>
+      <c r="M1" s="3"/>
+      <c r="N1" s="3"/>
+      <c r="O1" s="3"/>
+      <c r="P1" s="3"/>
+      <c r="Q1" s="3"/>
     </row>
     <row r="2" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A2" s="1" t="s">
@@ -745,195 +745,195 @@
       <c r="A3" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="B3" s="3" t="s">
+      <c r="B3" s="4" t="s">
         <v>22</v>
       </c>
-      <c r="C3" s="3"/>
-      <c r="D3" s="3"/>
-      <c r="E3" s="3"/>
-      <c r="F3" s="3" t="s">
+      <c r="C3" s="4"/>
+      <c r="D3" s="4"/>
+      <c r="E3" s="4"/>
+      <c r="F3" s="4" t="s">
         <v>23</v>
       </c>
-      <c r="G3" s="3"/>
-      <c r="H3" s="3"/>
-      <c r="I3" s="3"/>
-      <c r="J3" s="6" t="s">
+      <c r="G3" s="4"/>
+      <c r="H3" s="4"/>
+      <c r="I3" s="4"/>
+      <c r="J3" s="5" t="s">
         <v>24</v>
       </c>
-      <c r="K3" s="6"/>
-      <c r="L3" s="6"/>
-      <c r="M3" s="6"/>
-      <c r="N3" s="3" t="s">
+      <c r="K3" s="5"/>
+      <c r="L3" s="5"/>
+      <c r="M3" s="5"/>
+      <c r="N3" s="4" t="s">
         <v>25</v>
       </c>
-      <c r="O3" s="3"/>
-      <c r="P3" s="3"/>
-      <c r="Q3" s="3"/>
+      <c r="O3" s="4"/>
+      <c r="P3" s="4"/>
+      <c r="Q3" s="4"/>
     </row>
     <row r="4" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A4" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="B4" s="6" t="s">
+      <c r="B4" s="5" t="s">
         <v>24</v>
       </c>
-      <c r="C4" s="6"/>
-      <c r="D4" s="6"/>
-      <c r="E4" s="6"/>
-      <c r="F4" s="3" t="s">
+      <c r="C4" s="5"/>
+      <c r="D4" s="5"/>
+      <c r="E4" s="5"/>
+      <c r="F4" s="4" t="s">
         <v>26</v>
       </c>
-      <c r="G4" s="3"/>
-      <c r="H4" s="3"/>
-      <c r="I4" s="3"/>
-      <c r="J4" s="6" t="s">
+      <c r="G4" s="4"/>
+      <c r="H4" s="4"/>
+      <c r="I4" s="4"/>
+      <c r="J4" s="5" t="s">
         <v>24</v>
       </c>
-      <c r="K4" s="6"/>
-      <c r="L4" s="3" t="s">
+      <c r="K4" s="5"/>
+      <c r="L4" s="4" t="s">
         <v>27</v>
       </c>
-      <c r="M4" s="3"/>
-      <c r="N4" s="3"/>
-      <c r="O4" s="3"/>
-      <c r="P4" s="6" t="s">
+      <c r="M4" s="4"/>
+      <c r="N4" s="4"/>
+      <c r="O4" s="4"/>
+      <c r="P4" s="5" t="s">
         <v>24</v>
       </c>
-      <c r="Q4" s="6"/>
+      <c r="Q4" s="5"/>
     </row>
     <row r="5" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A5" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="B5" s="3" t="s">
+      <c r="B5" s="4" t="s">
         <v>28</v>
       </c>
-      <c r="C5" s="3"/>
-      <c r="D5" s="3"/>
-      <c r="E5" s="3"/>
+      <c r="C5" s="4"/>
+      <c r="D5" s="4"/>
+      <c r="E5" s="4"/>
       <c r="F5" s="7" t="s">
         <v>29</v>
       </c>
       <c r="G5" s="7"/>
       <c r="H5" s="7"/>
       <c r="I5" s="7"/>
-      <c r="J5" s="6" t="s">
+      <c r="J5" s="5" t="s">
         <v>24</v>
       </c>
-      <c r="K5" s="6"/>
-      <c r="L5" s="6"/>
-      <c r="M5" s="6"/>
-      <c r="N5" s="6"/>
-      <c r="O5" s="6"/>
-      <c r="P5" s="6"/>
-      <c r="Q5" s="6"/>
+      <c r="K5" s="5"/>
+      <c r="L5" s="5"/>
+      <c r="M5" s="5"/>
+      <c r="N5" s="5"/>
+      <c r="O5" s="5"/>
+      <c r="P5" s="5"/>
+      <c r="Q5" s="5"/>
     </row>
     <row r="6" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A6" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="B6" s="5" t="s">
+      <c r="B6" s="6" t="s">
         <v>34</v>
       </c>
-      <c r="C6" s="5"/>
-      <c r="D6" s="5"/>
-      <c r="E6" s="5"/>
-      <c r="F6" s="5"/>
-      <c r="G6" s="5"/>
-      <c r="H6" s="5"/>
-      <c r="I6" s="5"/>
-      <c r="J6" s="5"/>
-      <c r="K6" s="5"/>
-      <c r="L6" s="5"/>
-      <c r="M6" s="5"/>
-      <c r="N6" s="5"/>
-      <c r="O6" s="5"/>
-      <c r="P6" s="5"/>
-      <c r="Q6" s="5"/>
+      <c r="C6" s="6"/>
+      <c r="D6" s="6"/>
+      <c r="E6" s="6"/>
+      <c r="F6" s="6"/>
+      <c r="G6" s="6"/>
+      <c r="H6" s="6"/>
+      <c r="I6" s="6"/>
+      <c r="J6" s="6"/>
+      <c r="K6" s="6"/>
+      <c r="L6" s="6"/>
+      <c r="M6" s="6"/>
+      <c r="N6" s="6"/>
+      <c r="O6" s="6"/>
+      <c r="P6" s="6"/>
+      <c r="Q6" s="6"/>
     </row>
     <row r="7" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A7" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="B7" s="5"/>
-      <c r="C7" s="5"/>
-      <c r="D7" s="5"/>
-      <c r="E7" s="5"/>
-      <c r="F7" s="5"/>
-      <c r="G7" s="5"/>
-      <c r="H7" s="5"/>
-      <c r="I7" s="5"/>
-      <c r="J7" s="5"/>
-      <c r="K7" s="5"/>
-      <c r="L7" s="5"/>
-      <c r="M7" s="5"/>
-      <c r="N7" s="5"/>
-      <c r="O7" s="5"/>
-      <c r="P7" s="5"/>
-      <c r="Q7" s="5"/>
+      <c r="B7" s="6"/>
+      <c r="C7" s="6"/>
+      <c r="D7" s="6"/>
+      <c r="E7" s="6"/>
+      <c r="F7" s="6"/>
+      <c r="G7" s="6"/>
+      <c r="H7" s="6"/>
+      <c r="I7" s="6"/>
+      <c r="J7" s="6"/>
+      <c r="K7" s="6"/>
+      <c r="L7" s="6"/>
+      <c r="M7" s="6"/>
+      <c r="N7" s="6"/>
+      <c r="O7" s="6"/>
+      <c r="P7" s="6"/>
+      <c r="Q7" s="6"/>
     </row>
     <row r="8" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A8" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="B8" s="5"/>
-      <c r="C8" s="5"/>
-      <c r="D8" s="5"/>
-      <c r="E8" s="5"/>
-      <c r="F8" s="5"/>
-      <c r="G8" s="5"/>
-      <c r="H8" s="5"/>
-      <c r="I8" s="5"/>
-      <c r="J8" s="5"/>
-      <c r="K8" s="5"/>
-      <c r="L8" s="5"/>
-      <c r="M8" s="5"/>
-      <c r="N8" s="5"/>
-      <c r="O8" s="5"/>
-      <c r="P8" s="5"/>
-      <c r="Q8" s="5"/>
+      <c r="B8" s="6"/>
+      <c r="C8" s="6"/>
+      <c r="D8" s="6"/>
+      <c r="E8" s="6"/>
+      <c r="F8" s="6"/>
+      <c r="G8" s="6"/>
+      <c r="H8" s="6"/>
+      <c r="I8" s="6"/>
+      <c r="J8" s="6"/>
+      <c r="K8" s="6"/>
+      <c r="L8" s="6"/>
+      <c r="M8" s="6"/>
+      <c r="N8" s="6"/>
+      <c r="O8" s="6"/>
+      <c r="P8" s="6"/>
+      <c r="Q8" s="6"/>
     </row>
     <row r="9" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A9" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="B9" s="5" t="s">
+      <c r="B9" s="6" t="s">
         <v>36</v>
       </c>
-      <c r="C9" s="5"/>
-      <c r="D9" s="5"/>
-      <c r="E9" s="5"/>
-      <c r="F9" s="6" t="s">
+      <c r="C9" s="6"/>
+      <c r="D9" s="6"/>
+      <c r="E9" s="6"/>
+      <c r="F9" s="5" t="s">
         <v>24</v>
       </c>
-      <c r="G9" s="6"/>
-      <c r="H9" s="6"/>
-      <c r="I9" s="6"/>
-      <c r="J9" s="5" t="s">
+      <c r="G9" s="5"/>
+      <c r="H9" s="5"/>
+      <c r="I9" s="5"/>
+      <c r="J9" s="6" t="s">
         <v>37</v>
       </c>
-      <c r="K9" s="5"/>
-      <c r="L9" s="5"/>
-      <c r="M9" s="5"/>
-      <c r="N9" s="6" t="s">
+      <c r="K9" s="6"/>
+      <c r="L9" s="6"/>
+      <c r="M9" s="6"/>
+      <c r="N9" s="5" t="s">
         <v>24</v>
       </c>
-      <c r="O9" s="6"/>
-      <c r="P9" s="6"/>
-      <c r="Q9" s="6"/>
+      <c r="O9" s="5"/>
+      <c r="P9" s="5"/>
+      <c r="Q9" s="5"/>
     </row>
     <row r="10" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A10" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="B10" s="5" t="s">
+      <c r="B10" s="6" t="s">
         <v>38</v>
       </c>
-      <c r="C10" s="5"/>
-      <c r="D10" s="5" t="s">
+      <c r="C10" s="6"/>
+      <c r="D10" s="6" t="s">
         <v>39</v>
       </c>
-      <c r="E10" s="5"/>
+      <c r="E10" s="6"/>
       <c r="F10" s="2" t="s">
         <v>40</v>
       </c>
@@ -946,204 +946,205 @@
       <c r="I10" s="2" t="s">
         <v>43</v>
       </c>
-      <c r="J10" s="6" t="s">
+      <c r="J10" s="5" t="s">
         <v>24</v>
       </c>
-      <c r="K10" s="6"/>
-      <c r="L10" s="6"/>
-      <c r="M10" s="6"/>
-      <c r="N10" s="6"/>
-      <c r="O10" s="6"/>
-      <c r="P10" s="6"/>
-      <c r="Q10" s="6"/>
+      <c r="K10" s="5"/>
+      <c r="L10" s="5"/>
+      <c r="M10" s="5"/>
+      <c r="N10" s="5"/>
+      <c r="O10" s="5"/>
+      <c r="P10" s="5"/>
+      <c r="Q10" s="5"/>
     </row>
     <row r="11" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A11" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="B11" s="5" t="s">
+      <c r="B11" s="6" t="s">
         <v>35</v>
       </c>
-      <c r="C11" s="5"/>
-      <c r="D11" s="5"/>
-      <c r="E11" s="5"/>
-      <c r="F11" s="5"/>
-      <c r="G11" s="5"/>
-      <c r="H11" s="5"/>
-      <c r="I11" s="5"/>
-      <c r="J11" s="5"/>
-      <c r="K11" s="5"/>
-      <c r="L11" s="5"/>
-      <c r="M11" s="5"/>
-      <c r="N11" s="5"/>
-      <c r="O11" s="5"/>
-      <c r="P11" s="5"/>
-      <c r="Q11" s="5"/>
+      <c r="C11" s="6"/>
+      <c r="D11" s="6"/>
+      <c r="E11" s="6"/>
+      <c r="F11" s="6"/>
+      <c r="G11" s="6"/>
+      <c r="H11" s="6"/>
+      <c r="I11" s="6"/>
+      <c r="J11" s="6"/>
+      <c r="K11" s="6"/>
+      <c r="L11" s="6"/>
+      <c r="M11" s="6"/>
+      <c r="N11" s="6"/>
+      <c r="O11" s="6"/>
+      <c r="P11" s="6"/>
+      <c r="Q11" s="6"/>
     </row>
     <row r="12" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A12" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="B12" s="3" t="s">
+      <c r="B12" s="4" t="s">
         <v>44</v>
       </c>
-      <c r="C12" s="3"/>
-      <c r="D12" s="3"/>
-      <c r="E12" s="3"/>
-      <c r="F12" s="3"/>
-      <c r="G12" s="3"/>
-      <c r="H12" s="3"/>
-      <c r="I12" s="3"/>
-      <c r="J12" s="3"/>
-      <c r="K12" s="3"/>
-      <c r="L12" s="3"/>
-      <c r="M12" s="3"/>
-      <c r="N12" s="3"/>
-      <c r="O12" s="3"/>
-      <c r="P12" s="3"/>
-      <c r="Q12" s="3"/>
+      <c r="C12" s="4"/>
+      <c r="D12" s="4"/>
+      <c r="E12" s="4"/>
+      <c r="F12" s="4"/>
+      <c r="G12" s="4"/>
+      <c r="H12" s="4"/>
+      <c r="I12" s="4"/>
+      <c r="J12" s="4"/>
+      <c r="K12" s="4"/>
+      <c r="L12" s="4"/>
+      <c r="M12" s="4"/>
+      <c r="N12" s="4"/>
+      <c r="O12" s="4"/>
+      <c r="P12" s="4"/>
+      <c r="Q12" s="4"/>
     </row>
     <row r="13" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A13" s="1" t="s">
         <v>46</v>
       </c>
-      <c r="B13" s="3"/>
-      <c r="C13" s="3"/>
-      <c r="D13" s="3"/>
-      <c r="E13" s="3"/>
-      <c r="F13" s="3"/>
-      <c r="G13" s="3"/>
-      <c r="H13" s="3"/>
-      <c r="I13" s="3"/>
-      <c r="J13" s="3"/>
-      <c r="K13" s="3"/>
-      <c r="L13" s="3"/>
-      <c r="M13" s="3"/>
-      <c r="N13" s="3"/>
-      <c r="O13" s="3"/>
-      <c r="P13" s="3"/>
-      <c r="Q13" s="3"/>
+      <c r="B13" s="4"/>
+      <c r="C13" s="4"/>
+      <c r="D13" s="4"/>
+      <c r="E13" s="4"/>
+      <c r="F13" s="4"/>
+      <c r="G13" s="4"/>
+      <c r="H13" s="4"/>
+      <c r="I13" s="4"/>
+      <c r="J13" s="4"/>
+      <c r="K13" s="4"/>
+      <c r="L13" s="4"/>
+      <c r="M13" s="4"/>
+      <c r="N13" s="4"/>
+      <c r="O13" s="4"/>
+      <c r="P13" s="4"/>
+      <c r="Q13" s="4"/>
     </row>
     <row r="14" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A14" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="B14" s="3"/>
-      <c r="C14" s="3"/>
-      <c r="D14" s="3"/>
-      <c r="E14" s="3"/>
-      <c r="F14" s="3"/>
-      <c r="G14" s="3"/>
-      <c r="H14" s="3"/>
-      <c r="I14" s="3"/>
-      <c r="J14" s="3"/>
-      <c r="K14" s="3"/>
-      <c r="L14" s="3"/>
-      <c r="M14" s="3"/>
-      <c r="N14" s="3"/>
-      <c r="O14" s="3"/>
-      <c r="P14" s="3"/>
-      <c r="Q14" s="3"/>
+      <c r="B14" s="4"/>
+      <c r="C14" s="4"/>
+      <c r="D14" s="4"/>
+      <c r="E14" s="4"/>
+      <c r="F14" s="4"/>
+      <c r="G14" s="4"/>
+      <c r="H14" s="4"/>
+      <c r="I14" s="4"/>
+      <c r="J14" s="4"/>
+      <c r="K14" s="4"/>
+      <c r="L14" s="4"/>
+      <c r="M14" s="4"/>
+      <c r="N14" s="4"/>
+      <c r="O14" s="4"/>
+      <c r="P14" s="4"/>
+      <c r="Q14" s="4"/>
     </row>
     <row r="15" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A15" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="B15" s="3"/>
-      <c r="C15" s="3"/>
-      <c r="D15" s="3"/>
-      <c r="E15" s="3"/>
-      <c r="F15" s="3"/>
-      <c r="G15" s="3"/>
-      <c r="H15" s="3"/>
-      <c r="I15" s="3"/>
-      <c r="J15" s="3"/>
-      <c r="K15" s="3"/>
-      <c r="L15" s="3"/>
-      <c r="M15" s="3"/>
-      <c r="N15" s="3"/>
-      <c r="O15" s="3"/>
-      <c r="P15" s="3"/>
-      <c r="Q15" s="3"/>
+      <c r="B15" s="4"/>
+      <c r="C15" s="4"/>
+      <c r="D15" s="4"/>
+      <c r="E15" s="4"/>
+      <c r="F15" s="4"/>
+      <c r="G15" s="4"/>
+      <c r="H15" s="4"/>
+      <c r="I15" s="4"/>
+      <c r="J15" s="4"/>
+      <c r="K15" s="4"/>
+      <c r="L15" s="4"/>
+      <c r="M15" s="4"/>
+      <c r="N15" s="4"/>
+      <c r="O15" s="4"/>
+      <c r="P15" s="4"/>
+      <c r="Q15" s="4"/>
     </row>
     <row r="16" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A16" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="B16" s="3"/>
-      <c r="C16" s="3"/>
-      <c r="D16" s="3"/>
-      <c r="E16" s="3"/>
-      <c r="F16" s="3"/>
-      <c r="G16" s="3"/>
-      <c r="H16" s="3"/>
-      <c r="I16" s="3"/>
-      <c r="J16" s="3"/>
-      <c r="K16" s="3"/>
-      <c r="L16" s="3"/>
-      <c r="M16" s="3"/>
-      <c r="N16" s="3"/>
-      <c r="O16" s="3"/>
-      <c r="P16" s="3"/>
-      <c r="Q16" s="3"/>
+      <c r="B16" s="4"/>
+      <c r="C16" s="4"/>
+      <c r="D16" s="4"/>
+      <c r="E16" s="4"/>
+      <c r="F16" s="4"/>
+      <c r="G16" s="4"/>
+      <c r="H16" s="4"/>
+      <c r="I16" s="4"/>
+      <c r="J16" s="4"/>
+      <c r="K16" s="4"/>
+      <c r="L16" s="4"/>
+      <c r="M16" s="4"/>
+      <c r="N16" s="4"/>
+      <c r="O16" s="4"/>
+      <c r="P16" s="4"/>
+      <c r="Q16" s="4"/>
     </row>
     <row r="17" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A17" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="B17" s="3"/>
-      <c r="C17" s="3"/>
-      <c r="D17" s="3"/>
-      <c r="E17" s="3"/>
-      <c r="F17" s="3"/>
-      <c r="G17" s="3"/>
-      <c r="H17" s="3"/>
-      <c r="I17" s="3"/>
-      <c r="J17" s="3"/>
-      <c r="K17" s="3"/>
-      <c r="L17" s="3"/>
-      <c r="M17" s="3"/>
-      <c r="N17" s="3"/>
-      <c r="O17" s="3"/>
-      <c r="P17" s="3"/>
-      <c r="Q17" s="3"/>
+      <c r="B17" s="4"/>
+      <c r="C17" s="4"/>
+      <c r="D17" s="4"/>
+      <c r="E17" s="4"/>
+      <c r="F17" s="4"/>
+      <c r="G17" s="4"/>
+      <c r="H17" s="4"/>
+      <c r="I17" s="4"/>
+      <c r="J17" s="4"/>
+      <c r="K17" s="4"/>
+      <c r="L17" s="4"/>
+      <c r="M17" s="4"/>
+      <c r="N17" s="4"/>
+      <c r="O17" s="4"/>
+      <c r="P17" s="4"/>
+      <c r="Q17" s="4"/>
     </row>
     <row r="18" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A18" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="B18" s="3" t="s">
+      <c r="B18" s="4" t="s">
         <v>30</v>
       </c>
-      <c r="C18" s="3"/>
-      <c r="D18" s="3"/>
-      <c r="E18" s="3"/>
-      <c r="F18" s="3" t="s">
+      <c r="C18" s="4"/>
+      <c r="D18" s="4"/>
+      <c r="E18" s="4"/>
+      <c r="F18" s="4" t="s">
         <v>31</v>
       </c>
-      <c r="G18" s="3"/>
-      <c r="H18" s="3"/>
-      <c r="I18" s="3"/>
-      <c r="J18" s="3" t="s">
+      <c r="G18" s="4"/>
+      <c r="H18" s="4"/>
+      <c r="I18" s="4"/>
+      <c r="J18" s="4" t="s">
         <v>32</v>
       </c>
-      <c r="K18" s="3"/>
-      <c r="L18" s="3"/>
-      <c r="M18" s="3"/>
-      <c r="N18" s="3" t="s">
+      <c r="K18" s="4"/>
+      <c r="L18" s="4"/>
+      <c r="M18" s="4"/>
+      <c r="N18" s="4" t="s">
         <v>33</v>
       </c>
-      <c r="O18" s="3"/>
-      <c r="P18" s="3"/>
-      <c r="Q18" s="3"/>
+      <c r="O18" s="4"/>
+      <c r="P18" s="4"/>
+      <c r="Q18" s="4"/>
     </row>
   </sheetData>
   <mergeCells count="27">
-    <mergeCell ref="A1:Q1"/>
-    <mergeCell ref="B3:E3"/>
-    <mergeCell ref="F3:I3"/>
-    <mergeCell ref="J3:M3"/>
-    <mergeCell ref="N3:Q3"/>
+    <mergeCell ref="B12:Q17"/>
+    <mergeCell ref="F9:I9"/>
+    <mergeCell ref="J9:M9"/>
+    <mergeCell ref="N9:Q9"/>
+    <mergeCell ref="B10:C10"/>
+    <mergeCell ref="J10:Q10"/>
     <mergeCell ref="J5:Q5"/>
     <mergeCell ref="J18:M18"/>
     <mergeCell ref="N18:Q18"/>
@@ -1160,12 +1161,11 @@
     <mergeCell ref="B6:Q8"/>
     <mergeCell ref="D10:E10"/>
     <mergeCell ref="B9:E9"/>
-    <mergeCell ref="F9:I9"/>
-    <mergeCell ref="J9:M9"/>
-    <mergeCell ref="N9:Q9"/>
-    <mergeCell ref="B10:C10"/>
-    <mergeCell ref="J10:Q10"/>
-    <mergeCell ref="B12:Q17"/>
+    <mergeCell ref="A1:Q1"/>
+    <mergeCell ref="B3:E3"/>
+    <mergeCell ref="F3:I3"/>
+    <mergeCell ref="J3:M3"/>
+    <mergeCell ref="N3:Q3"/>
   </mergeCells>
   <phoneticPr fontId="4" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>